<commit_message>
een hoop gedaan, veel in het zorg gedeelte
</commit_message>
<xml_diff>
--- a/bestanden/lessentabellen_gc.xlsx
+++ b/bestanden/lessentabellen_gc.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GCvL\gcvl\bestanden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA869286-2EFF-4327-8F1C-57BE38ACBB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA3E097-5CC7-4324-87A1-F4B890D1A997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{138D59F3-F042-4F12-953E-758A0A5FA3B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="t" sheetId="1" r:id="rId1"/>
+    <sheet name="T" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="93">
   <si>
     <t>brugklas</t>
   </si>
@@ -176,9 +176,6 @@
     <t>aardrijkskunde</t>
   </si>
   <si>
-    <t>Mentoruur</t>
-  </si>
-  <si>
     <t>informatica</t>
   </si>
   <si>
@@ -248,9 +245,6 @@
     <t>beconomie</t>
   </si>
   <si>
-    <t>mentoruur</t>
-  </si>
-  <si>
     <t>handvaardigheid</t>
   </si>
   <si>
@@ -302,9 +296,6 @@
     <t>IT &amp; design</t>
   </si>
   <si>
-    <t>Mentoring</t>
-  </si>
-  <si>
     <t>mask</t>
   </si>
   <si>
@@ -321,6 +312,9 @@
   </si>
   <si>
     <t>2/3/4 mavo</t>
+  </si>
+  <si>
+    <t>Mentorles</t>
   </si>
 </sst>
 </file>
@@ -356,7 +350,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -894,26 +888,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -953,20 +932,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -975,31 +968,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1338,7 +1315,7 @@
   <dimension ref="A1:AS29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ12" sqref="AJ12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,191 +1341,191 @@
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="43"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="54"/>
+      <c r="F1" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="52"/>
       <c r="I1" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="56"/>
+      <c r="L1" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="52"/>
+      <c r="N1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="29" t="s">
+      <c r="O1" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="52"/>
+      <c r="T1" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="43"/>
-      <c r="T1" s="29" t="s">
+      <c r="V1" s="56"/>
+      <c r="W1" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" s="52"/>
+      <c r="AG1" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH1" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="V1" s="42"/>
-      <c r="W1" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="29" t="s">
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="Z1" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE1" s="43"/>
-      <c r="AG1" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH1" s="53" t="s">
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM1" s="53"/>
-      <c r="AN1" s="53"/>
-      <c r="AO1" s="53"/>
-      <c r="AP1" s="53" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="54"/>
+      <c r="AQ1" s="47"/>
+      <c r="AR1" s="47"/>
+      <c r="AS1" s="48"/>
     </row>
     <row r="2" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="28"/>
       <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="I2" s="28"/>
       <c r="J2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="L2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="N2" s="30"/>
       <c r="O2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="Q2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>52</v>
       </c>
       <c r="T2" s="28"/>
       <c r="U2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="W2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="36" t="s">
         <v>51</v>
-      </c>
-      <c r="X2" s="36" t="s">
-        <v>52</v>
       </c>
       <c r="Y2" s="28"/>
       <c r="Z2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="AB2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="AD2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="56" t="s">
+      <c r="AG2" s="43"/>
+      <c r="AH2" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK2" s="56"/>
-      <c r="AL2" s="56" t="s">
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56" t="s">
+      <c r="AO2" s="49"/>
+      <c r="AP2" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ2" s="49"/>
+      <c r="AR2" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS2" s="57"/>
+      <c r="AS2" s="50"/>
     </row>
     <row r="3" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -1603,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U3" s="2">
         <v>3</v>
@@ -1638,42 +1615,42 @@
       <c r="AE3" s="19">
         <v>2</v>
       </c>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI3" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ3" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK3" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL3" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="AM3" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="AN3" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO3" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="AP3" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="AQ3" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="AR3" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS3" s="60" t="s">
-        <v>86</v>
+      <c r="AG3" s="44"/>
+      <c r="AH3" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI3" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ3" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK3" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL3" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM3" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN3" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO3" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP3" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ3" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR3" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS3" s="46" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
@@ -1729,7 +1706,7 @@
         <v>2</v>
       </c>
       <c r="T4" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U4" s="2">
         <v>2</v>
@@ -1767,30 +1744,30 @@
       <c r="AG4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" s="48">
-        <v>3</v>
-      </c>
-      <c r="AI4" s="48"/>
-      <c r="AJ4" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK4" s="48"/>
-      <c r="AL4" s="48">
-        <v>2</v>
-      </c>
-      <c r="AM4" s="48"/>
-      <c r="AN4" s="48">
-        <v>2</v>
-      </c>
-      <c r="AO4" s="48"/>
-      <c r="AP4" s="48">
-        <v>3</v>
-      </c>
-      <c r="AQ4" s="48"/>
-      <c r="AR4" s="48">
-        <v>3</v>
-      </c>
-      <c r="AS4" s="49"/>
+      <c r="AH4" s="40">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="40"/>
+      <c r="AJ4" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK4" s="40"/>
+      <c r="AL4" s="40">
+        <v>2</v>
+      </c>
+      <c r="AM4" s="40"/>
+      <c r="AN4" s="40">
+        <v>2</v>
+      </c>
+      <c r="AO4" s="40"/>
+      <c r="AP4" s="40">
+        <v>3</v>
+      </c>
+      <c r="AQ4" s="40"/>
+      <c r="AR4" s="40">
+        <v>3</v>
+      </c>
+      <c r="AS4" s="41"/>
     </row>
     <row r="5" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
@@ -1835,7 +1812,7 @@
         <v>2</v>
       </c>
       <c r="T5" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U5" s="2">
         <v>2</v>
@@ -1873,28 +1850,28 @@
       <c r="AG5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="48">
-        <v>3</v>
-      </c>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48">
-        <v>2</v>
-      </c>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN5" s="48"/>
-      <c r="AO5" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP5" s="48"/>
-      <c r="AQ5" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR5" s="48"/>
-      <c r="AS5" s="49">
+      <c r="AH5" s="40"/>
+      <c r="AI5" s="40">
+        <v>3</v>
+      </c>
+      <c r="AJ5" s="40"/>
+      <c r="AK5" s="40">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="40"/>
+      <c r="AM5" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="40"/>
+      <c r="AO5" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP5" s="40"/>
+      <c r="AQ5" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR5" s="40"/>
+      <c r="AS5" s="41">
         <v>3</v>
       </c>
     </row>
@@ -1951,7 +1928,7 @@
         <v>2</v>
       </c>
       <c r="T6" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U6" s="2">
         <v>2</v>
@@ -1989,28 +1966,28 @@
       <c r="AG6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AH6" s="48"/>
-      <c r="AI6" s="48">
-        <v>3</v>
-      </c>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48">
-        <v>2</v>
-      </c>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN6" s="48"/>
-      <c r="AO6" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP6" s="48"/>
-      <c r="AQ6" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR6" s="48"/>
-      <c r="AS6" s="49">
+      <c r="AH6" s="40"/>
+      <c r="AI6" s="40">
+        <v>3</v>
+      </c>
+      <c r="AJ6" s="40"/>
+      <c r="AK6" s="40">
+        <v>2</v>
+      </c>
+      <c r="AL6" s="40"/>
+      <c r="AM6" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN6" s="40"/>
+      <c r="AO6" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP6" s="40"/>
+      <c r="AQ6" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR6" s="40"/>
+      <c r="AS6" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2087,30 +2064,30 @@
       <c r="AG7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="AH7" s="48">
-        <v>3</v>
-      </c>
-      <c r="AI7" s="48"/>
-      <c r="AJ7" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK7" s="48"/>
-      <c r="AL7" s="48">
-        <v>2</v>
-      </c>
-      <c r="AM7" s="48"/>
-      <c r="AN7" s="48">
-        <v>2</v>
-      </c>
-      <c r="AO7" s="48"/>
-      <c r="AP7" s="48">
-        <v>3</v>
-      </c>
-      <c r="AQ7" s="48"/>
-      <c r="AR7" s="48">
-        <v>3</v>
-      </c>
-      <c r="AS7" s="49"/>
+      <c r="AH7" s="40">
+        <v>3</v>
+      </c>
+      <c r="AI7" s="40"/>
+      <c r="AJ7" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK7" s="40"/>
+      <c r="AL7" s="40">
+        <v>2</v>
+      </c>
+      <c r="AM7" s="40"/>
+      <c r="AN7" s="40">
+        <v>2</v>
+      </c>
+      <c r="AO7" s="40"/>
+      <c r="AP7" s="40">
+        <v>3</v>
+      </c>
+      <c r="AQ7" s="40"/>
+      <c r="AR7" s="40">
+        <v>3</v>
+      </c>
+      <c r="AS7" s="41"/>
     </row>
     <row r="8" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -2174,7 +2151,7 @@
         <v>2</v>
       </c>
       <c r="Y8" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z8" s="2">
         <v>2</v>
@@ -2197,26 +2174,26 @@
       <c r="AG8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="AH8" s="48">
-        <v>3</v>
-      </c>
-      <c r="AI8" s="48"/>
-      <c r="AJ8" s="48"/>
-      <c r="AK8" s="48"/>
-      <c r="AL8" s="48"/>
-      <c r="AM8" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN8" s="48"/>
-      <c r="AO8" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP8" s="48"/>
-      <c r="AQ8" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR8" s="48"/>
-      <c r="AS8" s="49">
+      <c r="AH8" s="40">
+        <v>3</v>
+      </c>
+      <c r="AI8" s="40"/>
+      <c r="AJ8" s="40"/>
+      <c r="AK8" s="40"/>
+      <c r="AL8" s="40"/>
+      <c r="AM8" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN8" s="40"/>
+      <c r="AO8" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="40"/>
+      <c r="AQ8" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR8" s="40"/>
+      <c r="AS8" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2282,7 +2259,7 @@
         <v>3</v>
       </c>
       <c r="Y9" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Z9" s="2">
         <v>2</v>
@@ -2305,28 +2282,28 @@
       <c r="AG9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="AH9" s="48">
-        <v>2</v>
-      </c>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="48">
-        <v>1</v>
-      </c>
-      <c r="AK9" s="48"/>
-      <c r="AL9" s="48"/>
-      <c r="AM9" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN9" s="48"/>
-      <c r="AO9" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP9" s="48"/>
-      <c r="AQ9" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR9" s="48"/>
-      <c r="AS9" s="49">
+      <c r="AH9" s="40">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="40"/>
+      <c r="AJ9" s="40">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="40"/>
+      <c r="AL9" s="40"/>
+      <c r="AM9" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN9" s="40"/>
+      <c r="AO9" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP9" s="40"/>
+      <c r="AQ9" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR9" s="40"/>
+      <c r="AS9" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2398,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="Y10" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z10" s="2">
         <v>2</v>
@@ -2421,28 +2398,28 @@
       <c r="AG10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="AH10" s="48">
-        <v>2</v>
-      </c>
-      <c r="AI10" s="48"/>
-      <c r="AJ10" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK10" s="48"/>
-      <c r="AL10" s="48">
-        <v>2</v>
-      </c>
-      <c r="AM10" s="48"/>
-      <c r="AN10" s="48">
-        <v>2</v>
-      </c>
-      <c r="AO10" s="48"/>
-      <c r="AP10" s="48"/>
-      <c r="AQ10" s="48">
+      <c r="AH10" s="40">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="40"/>
+      <c r="AJ10" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK10" s="40"/>
+      <c r="AL10" s="40">
+        <v>2</v>
+      </c>
+      <c r="AM10" s="40"/>
+      <c r="AN10" s="40">
+        <v>2</v>
+      </c>
+      <c r="AO10" s="40"/>
+      <c r="AP10" s="40"/>
+      <c r="AQ10" s="40">
         <v>4</v>
       </c>
-      <c r="AR10" s="48"/>
-      <c r="AS10" s="49">
+      <c r="AR10" s="40"/>
+      <c r="AS10" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2529,28 +2506,28 @@
       <c r="AG11" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="AH11" s="48">
-        <v>2</v>
-      </c>
-      <c r="AI11" s="48"/>
-      <c r="AJ11" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK11" s="48"/>
-      <c r="AL11" s="48"/>
-      <c r="AM11" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN11" s="48"/>
-      <c r="AO11" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP11" s="48"/>
-      <c r="AQ11" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR11" s="48"/>
-      <c r="AS11" s="49">
+      <c r="AH11" s="40">
+        <v>2</v>
+      </c>
+      <c r="AI11" s="40"/>
+      <c r="AJ11" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK11" s="40"/>
+      <c r="AL11" s="40"/>
+      <c r="AM11" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN11" s="40"/>
+      <c r="AO11" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP11" s="40"/>
+      <c r="AQ11" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR11" s="40"/>
+      <c r="AS11" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2637,26 +2614,26 @@
       <c r="AG12" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="AH12" s="48"/>
-      <c r="AI12" s="48"/>
-      <c r="AJ12" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK12" s="48"/>
-      <c r="AL12" s="48"/>
-      <c r="AM12" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN12" s="48"/>
-      <c r="AO12" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP12" s="48"/>
-      <c r="AQ12" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR12" s="48"/>
-      <c r="AS12" s="49">
+      <c r="AH12" s="40"/>
+      <c r="AI12" s="40"/>
+      <c r="AJ12" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK12" s="40"/>
+      <c r="AL12" s="40"/>
+      <c r="AM12" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN12" s="40"/>
+      <c r="AO12" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP12" s="40"/>
+      <c r="AQ12" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR12" s="40"/>
+      <c r="AS12" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2688,7 +2665,7 @@
         <v>1</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O13" s="2">
         <v>2</v>
@@ -2737,24 +2714,24 @@
       <c r="AG13" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="AH13" s="48"/>
-      <c r="AI13" s="48"/>
-      <c r="AJ13" s="48"/>
-      <c r="AK13" s="48"/>
-      <c r="AL13" s="48"/>
-      <c r="AM13" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN13" s="48"/>
-      <c r="AO13" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP13" s="48"/>
-      <c r="AQ13" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR13" s="48"/>
-      <c r="AS13" s="49">
+      <c r="AH13" s="40"/>
+      <c r="AI13" s="40"/>
+      <c r="AJ13" s="40"/>
+      <c r="AK13" s="40"/>
+      <c r="AL13" s="40"/>
+      <c r="AM13" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="40"/>
+      <c r="AO13" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP13" s="40"/>
+      <c r="AQ13" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR13" s="40"/>
+      <c r="AS13" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2784,7 +2761,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O14" s="2">
         <v>3</v>
@@ -2799,7 +2776,7 @@
         <v>2</v>
       </c>
       <c r="T14" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2">
@@ -2810,7 +2787,7 @@
       </c>
       <c r="X14" s="9"/>
       <c r="Y14" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Z14" s="2">
         <v>1</v>
@@ -2833,28 +2810,28 @@
       <c r="AG14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="AH14" s="48">
-        <v>1</v>
-      </c>
-      <c r="AI14" s="48"/>
-      <c r="AJ14" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK14" s="48"/>
-      <c r="AL14" s="48"/>
-      <c r="AM14" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN14" s="48"/>
-      <c r="AO14" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP14" s="48"/>
-      <c r="AQ14" s="48">
+      <c r="AH14" s="40">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="40"/>
+      <c r="AJ14" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK14" s="40"/>
+      <c r="AL14" s="40"/>
+      <c r="AM14" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN14" s="40"/>
+      <c r="AO14" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP14" s="40"/>
+      <c r="AQ14" s="40">
         <v>4</v>
       </c>
-      <c r="AR14" s="48"/>
-      <c r="AS14" s="49">
+      <c r="AR14" s="40"/>
+      <c r="AS14" s="41">
         <v>3</v>
       </c>
     </row>
@@ -2907,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="T15" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U15" s="2">
         <v>1</v>
@@ -2941,20 +2918,20 @@
       <c r="AG15" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="AH15" s="48"/>
-      <c r="AI15" s="48"/>
-      <c r="AJ15" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK15" s="48"/>
-      <c r="AL15" s="48"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="48"/>
-      <c r="AO15" s="48"/>
-      <c r="AP15" s="48"/>
-      <c r="AQ15" s="48"/>
-      <c r="AR15" s="48"/>
-      <c r="AS15" s="49"/>
+      <c r="AH15" s="40"/>
+      <c r="AI15" s="40"/>
+      <c r="AJ15" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK15" s="40"/>
+      <c r="AL15" s="40"/>
+      <c r="AM15" s="40"/>
+      <c r="AN15" s="40"/>
+      <c r="AO15" s="40"/>
+      <c r="AP15" s="40"/>
+      <c r="AQ15" s="40"/>
+      <c r="AR15" s="40"/>
+      <c r="AS15" s="41"/>
     </row>
     <row r="16" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
@@ -3045,26 +3022,26 @@
         <v>2</v>
       </c>
       <c r="AG16" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH16" s="48"/>
-      <c r="AI16" s="48"/>
-      <c r="AJ16" s="48"/>
-      <c r="AK16" s="48"/>
-      <c r="AL16" s="48"/>
-      <c r="AM16" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN16" s="48"/>
-      <c r="AO16" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP16" s="48"/>
-      <c r="AQ16" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR16" s="48"/>
-      <c r="AS16" s="49">
+        <v>85</v>
+      </c>
+      <c r="AH16" s="40"/>
+      <c r="AI16" s="40"/>
+      <c r="AJ16" s="40"/>
+      <c r="AK16" s="40"/>
+      <c r="AL16" s="40"/>
+      <c r="AM16" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN16" s="40"/>
+      <c r="AO16" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP16" s="40"/>
+      <c r="AQ16" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR16" s="40"/>
+      <c r="AS16" s="41">
         <v>2</v>
       </c>
     </row>
@@ -3157,30 +3134,30 @@
         <v>2</v>
       </c>
       <c r="AG17" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH17" s="48">
-        <v>2</v>
-      </c>
-      <c r="AI17" s="48"/>
-      <c r="AJ17" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK17" s="48"/>
-      <c r="AL17" s="48"/>
-      <c r="AM17" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN17" s="48"/>
-      <c r="AO17" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP17" s="48"/>
-      <c r="AQ17" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR17" s="48"/>
-      <c r="AS17" s="49">
+        <v>69</v>
+      </c>
+      <c r="AH17" s="40">
+        <v>2</v>
+      </c>
+      <c r="AI17" s="40"/>
+      <c r="AJ17" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK17" s="40"/>
+      <c r="AL17" s="40"/>
+      <c r="AM17" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN17" s="40"/>
+      <c r="AO17" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP17" s="40"/>
+      <c r="AQ17" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR17" s="40"/>
+      <c r="AS17" s="41">
         <v>3</v>
       </c>
     </row>
@@ -3233,22 +3210,22 @@
         <v>2</v>
       </c>
       <c r="T18" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="U18" s="2">
+        <v>2</v>
+      </c>
+      <c r="V18" s="2">
+        <v>2</v>
+      </c>
+      <c r="W18" s="2">
+        <v>2</v>
+      </c>
+      <c r="X18" s="9">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="U18" s="2">
-        <v>2</v>
-      </c>
-      <c r="V18" s="2">
-        <v>2</v>
-      </c>
-      <c r="W18" s="2">
-        <v>2</v>
-      </c>
-      <c r="X18" s="9">
-        <v>2</v>
-      </c>
-      <c r="Y18" s="18" t="s">
-        <v>69</v>
       </c>
       <c r="Z18" s="2">
         <v>2</v>
@@ -3271,28 +3248,28 @@
       <c r="AG18" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="AH18" s="48">
-        <v>1</v>
-      </c>
-      <c r="AI18" s="48"/>
-      <c r="AJ18" s="48">
-        <v>1</v>
-      </c>
-      <c r="AK18" s="48"/>
-      <c r="AL18" s="48"/>
-      <c r="AM18" s="48">
-        <v>2</v>
-      </c>
-      <c r="AN18" s="48"/>
-      <c r="AO18" s="48">
-        <v>2</v>
-      </c>
-      <c r="AP18" s="48"/>
-      <c r="AQ18" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR18" s="48"/>
-      <c r="AS18" s="49">
+      <c r="AH18" s="40">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="40"/>
+      <c r="AJ18" s="40">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="40"/>
+      <c r="AL18" s="40"/>
+      <c r="AM18" s="40">
+        <v>2</v>
+      </c>
+      <c r="AN18" s="40"/>
+      <c r="AO18" s="40">
+        <v>2</v>
+      </c>
+      <c r="AP18" s="40"/>
+      <c r="AQ18" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR18" s="40"/>
+      <c r="AS18" s="41">
         <v>3</v>
       </c>
     </row>
@@ -3319,13 +3296,13 @@
         <v>2</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="J19" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K19" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L19" s="2">
         <v>0.5</v>
@@ -3334,7 +3311,7 @@
         <v>0.5</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O19" s="2">
         <v>2</v>
@@ -3349,7 +3326,7 @@
         <v>2</v>
       </c>
       <c r="T19" s="31" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="U19" s="2">
         <v>0.5</v>
@@ -3387,28 +3364,28 @@
       <c r="AG19" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="AH19" s="48"/>
-      <c r="AI19" s="48"/>
-      <c r="AJ19" s="48">
-        <v>2</v>
-      </c>
-      <c r="AK19" s="48"/>
-      <c r="AL19" s="48">
-        <v>2</v>
-      </c>
-      <c r="AM19" s="48"/>
-      <c r="AN19" s="48">
-        <v>3</v>
-      </c>
-      <c r="AO19" s="48"/>
-      <c r="AP19" s="48"/>
-      <c r="AQ19" s="48"/>
-      <c r="AR19" s="48"/>
-      <c r="AS19" s="49"/>
+      <c r="AH19" s="40"/>
+      <c r="AI19" s="40"/>
+      <c r="AJ19" s="40">
+        <v>2</v>
+      </c>
+      <c r="AK19" s="40"/>
+      <c r="AL19" s="40">
+        <v>2</v>
+      </c>
+      <c r="AM19" s="40"/>
+      <c r="AN19" s="40">
+        <v>3</v>
+      </c>
+      <c r="AO19" s="40"/>
+      <c r="AP19" s="40"/>
+      <c r="AQ19" s="40"/>
+      <c r="AR19" s="40"/>
+      <c r="AS19" s="41"/>
     </row>
     <row r="20" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
@@ -3429,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" s="2">
         <v>1</v>
@@ -3459,7 +3436,7 @@
         <v>2</v>
       </c>
       <c r="T20" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U20" s="2">
         <v>2</v>
@@ -3474,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="Y20" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z20" s="2">
         <v>1</v>
@@ -3495,32 +3472,32 @@
         <v>1</v>
       </c>
       <c r="AG20" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH20" s="48">
-        <v>1</v>
-      </c>
-      <c r="AI20" s="48"/>
-      <c r="AJ20" s="48">
-        <v>1</v>
-      </c>
-      <c r="AK20" s="48"/>
-      <c r="AL20" s="48">
-        <v>1</v>
-      </c>
-      <c r="AM20" s="48"/>
-      <c r="AN20" s="48">
-        <v>1</v>
-      </c>
-      <c r="AO20" s="48"/>
-      <c r="AP20" s="48">
+        <v>27</v>
+      </c>
+      <c r="AH20" s="40">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="40"/>
+      <c r="AJ20" s="40">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="40"/>
+      <c r="AL20" s="40">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="40"/>
+      <c r="AN20" s="40">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="40"/>
+      <c r="AP20" s="40">
         <v>0.5</v>
       </c>
-      <c r="AQ20" s="48"/>
-      <c r="AR20" s="48">
+      <c r="AQ20" s="40"/>
+      <c r="AR20" s="40">
         <v>0.5</v>
       </c>
-      <c r="AS20" s="49"/>
+      <c r="AS20" s="41"/>
     </row>
     <row r="21" spans="1:45" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="24" t="s">
@@ -3554,15 +3531,19 @@
         <v>16</v>
       </c>
       <c r="J21" s="25">
-        <v>25</v>
+        <f>SUM(J3:J20)</f>
+        <v>24.5</v>
       </c>
       <c r="K21" s="25">
-        <v>27</v>
+        <f t="shared" ref="K21:M21" si="1">SUM(K3:K20)</f>
+        <v>26.5</v>
       </c>
       <c r="L21" s="25">
+        <f t="shared" si="1"/>
         <v>27.5</v>
       </c>
-      <c r="M21" s="26">
+      <c r="M21" s="25">
+        <f t="shared" si="1"/>
         <v>27.5</v>
       </c>
       <c r="N21" s="18" t="s">
@@ -3617,22 +3598,22 @@
         <v>2</v>
       </c>
       <c r="AG21" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH21" s="48"/>
-      <c r="AI21" s="48"/>
-      <c r="AJ21" s="48"/>
-      <c r="AK21" s="48"/>
-      <c r="AL21" s="48"/>
-      <c r="AM21" s="48"/>
-      <c r="AN21" s="48"/>
-      <c r="AO21" s="48"/>
-      <c r="AP21" s="48"/>
-      <c r="AQ21" s="48">
-        <v>3</v>
-      </c>
-      <c r="AR21" s="48"/>
-      <c r="AS21" s="49">
+        <v>86</v>
+      </c>
+      <c r="AH21" s="40"/>
+      <c r="AI21" s="40"/>
+      <c r="AJ21" s="40"/>
+      <c r="AK21" s="40"/>
+      <c r="AL21" s="40"/>
+      <c r="AM21" s="40"/>
+      <c r="AN21" s="40"/>
+      <c r="AO21" s="40"/>
+      <c r="AP21" s="40"/>
+      <c r="AQ21" s="40">
+        <v>3</v>
+      </c>
+      <c r="AR21" s="40"/>
+      <c r="AS21" s="41">
         <v>3</v>
       </c>
     </row>
@@ -3643,7 +3624,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O22" s="2">
         <v>2</v>
@@ -3658,7 +3639,7 @@
         <v>2</v>
       </c>
       <c r="T22" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U22" s="12">
         <f>SUM(U3:U20)</f>
@@ -3698,20 +3679,20 @@
       <c r="AG22" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AH22" s="48">
-        <v>1</v>
-      </c>
-      <c r="AI22" s="48"/>
-      <c r="AJ22" s="48"/>
-      <c r="AK22" s="48"/>
-      <c r="AL22" s="48"/>
-      <c r="AM22" s="48"/>
-      <c r="AN22" s="48"/>
-      <c r="AO22" s="48"/>
-      <c r="AP22" s="48"/>
-      <c r="AQ22" s="48"/>
-      <c r="AR22" s="48"/>
-      <c r="AS22" s="49"/>
+      <c r="AH22" s="40">
+        <v>1</v>
+      </c>
+      <c r="AI22" s="40"/>
+      <c r="AJ22" s="40"/>
+      <c r="AK22" s="40"/>
+      <c r="AL22" s="40"/>
+      <c r="AM22" s="40"/>
+      <c r="AN22" s="40"/>
+      <c r="AO22" s="40"/>
+      <c r="AP22" s="40"/>
+      <c r="AQ22" s="40"/>
+      <c r="AR22" s="40"/>
+      <c r="AS22" s="41"/>
     </row>
     <row r="23" spans="1:45" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I23" s="7"/>
@@ -3720,7 +3701,7 @@
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O23" s="21">
         <v>7</v>
@@ -3735,7 +3716,7 @@
         <v>8</v>
       </c>
       <c r="T23" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U23" s="14"/>
       <c r="V23" s="13"/>
@@ -3746,7 +3727,7 @@
         <v>25.5</v>
       </c>
       <c r="Y23" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2">
@@ -3761,34 +3742,34 @@
       <c r="AG23" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="AH23" s="48">
-        <v>2</v>
-      </c>
-      <c r="AI23" s="48"/>
-      <c r="AJ23" s="48">
-        <v>3</v>
-      </c>
-      <c r="AK23" s="48"/>
-      <c r="AL23" s="48">
-        <v>2</v>
-      </c>
-      <c r="AM23" s="48"/>
-      <c r="AN23" s="48">
-        <v>2</v>
-      </c>
-      <c r="AO23" s="48"/>
-      <c r="AP23" s="48">
+      <c r="AH23" s="40">
+        <v>2</v>
+      </c>
+      <c r="AI23" s="40"/>
+      <c r="AJ23" s="40">
+        <v>3</v>
+      </c>
+      <c r="AK23" s="40"/>
+      <c r="AL23" s="40">
+        <v>2</v>
+      </c>
+      <c r="AM23" s="40"/>
+      <c r="AN23" s="40">
+        <v>2</v>
+      </c>
+      <c r="AO23" s="40"/>
+      <c r="AP23" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="AQ23" s="48"/>
-      <c r="AR23" s="48">
+      <c r="AQ23" s="40"/>
+      <c r="AR23" s="40">
         <v>1.1299999999999999</v>
       </c>
-      <c r="AS23" s="49"/>
+      <c r="AS23" s="41"/>
     </row>
     <row r="24" spans="1:45" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T24" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="U24" s="35"/>
       <c r="V24" s="21"/>
@@ -3799,7 +3780,7 @@
         <v>26.5</v>
       </c>
       <c r="Y24" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Z24" s="13">
         <v>2</v>
@@ -3820,31 +3801,31 @@
         <v>0.75</v>
       </c>
       <c r="AG24" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH24" s="48"/>
-      <c r="AI24" s="48"/>
-      <c r="AJ24" s="48"/>
-      <c r="AK24" s="48"/>
-      <c r="AL24" s="48">
-        <v>1</v>
-      </c>
-      <c r="AM24" s="48"/>
-      <c r="AN24" s="48"/>
-      <c r="AO24" s="48"/>
-      <c r="AP24" s="48"/>
-      <c r="AQ24" s="48"/>
-      <c r="AR24" s="48"/>
-      <c r="AS24" s="49"/>
+        <v>71</v>
+      </c>
+      <c r="AH24" s="40"/>
+      <c r="AI24" s="40"/>
+      <c r="AJ24" s="40"/>
+      <c r="AK24" s="40"/>
+      <c r="AL24" s="40">
+        <v>1</v>
+      </c>
+      <c r="AM24" s="40"/>
+      <c r="AN24" s="40"/>
+      <c r="AO24" s="40"/>
+      <c r="AP24" s="40"/>
+      <c r="AQ24" s="40"/>
+      <c r="AR24" s="40"/>
+      <c r="AS24" s="41"/>
     </row>
     <row r="25" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="T25" s="1"/>
-      <c r="U25" s="39"/>
-      <c r="V25" s="39"/>
-      <c r="W25" s="39"/>
-      <c r="X25" s="39"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
       <c r="Y25" s="18" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="Z25" s="2">
         <v>1</v>
@@ -3865,31 +3846,31 @@
         <v>1</v>
       </c>
       <c r="AG25" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH25" s="48"/>
-      <c r="AI25" s="48"/>
-      <c r="AJ25" s="48">
-        <v>1</v>
-      </c>
-      <c r="AK25" s="48"/>
-      <c r="AL25" s="48"/>
-      <c r="AM25" s="48"/>
-      <c r="AN25" s="48"/>
-      <c r="AO25" s="48"/>
-      <c r="AP25" s="48"/>
-      <c r="AQ25" s="48"/>
-      <c r="AR25" s="48"/>
-      <c r="AS25" s="49"/>
+        <v>90</v>
+      </c>
+      <c r="AH25" s="40"/>
+      <c r="AI25" s="40"/>
+      <c r="AJ25" s="40">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="40"/>
+      <c r="AL25" s="40"/>
+      <c r="AM25" s="40"/>
+      <c r="AN25" s="40"/>
+      <c r="AO25" s="40"/>
+      <c r="AP25" s="40"/>
+      <c r="AQ25" s="40"/>
+      <c r="AR25" s="40"/>
+      <c r="AS25" s="41"/>
     </row>
     <row r="26" spans="1:45" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T26" s="1"/>
-      <c r="U26" s="39"/>
-      <c r="V26" s="39"/>
-      <c r="W26" s="39"/>
-      <c r="X26" s="39"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
       <c r="Y26" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Z26" s="21">
         <v>7</v>
@@ -3912,83 +3893,105 @@
       <c r="AG26" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AH26" s="48"/>
-      <c r="AI26" s="48"/>
-      <c r="AJ26" s="48"/>
-      <c r="AK26" s="48"/>
-      <c r="AL26" s="48">
-        <v>2</v>
-      </c>
-      <c r="AM26" s="48"/>
-      <c r="AN26" s="48">
-        <v>2</v>
-      </c>
-      <c r="AO26" s="48"/>
-      <c r="AP26" s="48"/>
-      <c r="AQ26" s="48"/>
-      <c r="AR26" s="48"/>
-      <c r="AS26" s="49"/>
+      <c r="AH26" s="40"/>
+      <c r="AI26" s="40"/>
+      <c r="AJ26" s="40"/>
+      <c r="AK26" s="40"/>
+      <c r="AL26" s="40">
+        <v>2</v>
+      </c>
+      <c r="AM26" s="40"/>
+      <c r="AN26" s="40">
+        <v>2</v>
+      </c>
+      <c r="AO26" s="40"/>
+      <c r="AP26" s="40"/>
+      <c r="AQ26" s="40"/>
+      <c r="AR26" s="40"/>
+      <c r="AS26" s="41"/>
     </row>
     <row r="27" spans="1:45" ht="15.6" x14ac:dyDescent="0.3">
       <c r="AG27" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH27" s="48"/>
-      <c r="AI27" s="48"/>
-      <c r="AJ27" s="48"/>
-      <c r="AK27" s="48"/>
-      <c r="AL27" s="48"/>
-      <c r="AM27" s="48"/>
-      <c r="AN27" s="48"/>
-      <c r="AO27" s="48"/>
-      <c r="AP27" s="48">
-        <v>1</v>
-      </c>
-      <c r="AQ27" s="48"/>
-      <c r="AR27" s="48">
-        <v>1</v>
-      </c>
-      <c r="AS27" s="49"/>
+        <v>87</v>
+      </c>
+      <c r="AH27" s="40"/>
+      <c r="AI27" s="40"/>
+      <c r="AJ27" s="40"/>
+      <c r="AK27" s="40"/>
+      <c r="AL27" s="40"/>
+      <c r="AM27" s="40"/>
+      <c r="AN27" s="40"/>
+      <c r="AO27" s="40"/>
+      <c r="AP27" s="40">
+        <v>1</v>
+      </c>
+      <c r="AQ27" s="40"/>
+      <c r="AR27" s="40">
+        <v>1</v>
+      </c>
+      <c r="AS27" s="41"/>
     </row>
     <row r="28" spans="1:45" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AG28" s="47" t="s">
+      <c r="AG28" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="AH28" s="50">
+      <c r="AH28" s="42">
+        <f>SUM(AH4:AH27)</f>
         <v>23</v>
       </c>
-      <c r="AI28" s="50"/>
-      <c r="AJ28" s="50">
-        <v>27</v>
-      </c>
-      <c r="AK28" s="50"/>
-      <c r="AL28" s="50">
+      <c r="AI28" s="42"/>
+      <c r="AJ28" s="42">
+        <f t="shared" ref="AI28:AS28" si="2">SUM(AJ4:AJ27)</f>
+        <v>25</v>
+      </c>
+      <c r="AK28" s="42"/>
+      <c r="AL28" s="42">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="AM28" s="50"/>
-      <c r="AN28" s="50">
-        <v>16</v>
-      </c>
-      <c r="AO28" s="50"/>
-      <c r="AP28" s="50">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="AQ28" s="50"/>
-      <c r="AR28" s="50">
-        <v>11.63</v>
-      </c>
-      <c r="AS28" s="51"/>
+      <c r="AM28" s="42"/>
+      <c r="AN28" s="42">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="AO28" s="42"/>
+      <c r="AP28" s="42">
+        <f t="shared" si="2"/>
+        <v>8.629999999999999</v>
+      </c>
+      <c r="AQ28" s="42"/>
+      <c r="AR28" s="42">
+        <f t="shared" si="2"/>
+        <v>8.629999999999999</v>
+      </c>
+      <c r="AS28" s="42"/>
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="AH29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AK29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="AP1:AS1"/>
@@ -3998,22 +4001,6 @@
     <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="AP2:AQ2"/>
     <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>